<commit_message>
Tried to include a macro, not sure if it worked
Did a macro for select/deselecting all of the boxes for a page. But im not sure if it worked. I dont think the fileformat allows to save macros.
</commit_message>
<xml_diff>
--- a/mainProcedure.xlsx
+++ b/mainProcedure.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexandragustafsson/Documents/TCRYA-civ.ing/RAVEN - som inte finns på teams/RavenProcedure/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3602A94F-0402-674F-A505-2AB8EE7B4120}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7639619B-CF93-F74C-BD68-CB709C058C81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="540" windowWidth="35840" windowHeight="21860" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mainProcedure" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="260">
   <si>
     <t>Version</t>
   </si>
@@ -963,12 +963,15 @@
   <si>
     <t xml:space="preserve">The checking have to be done sequentially to ensure the systems works in the correct way and all steps are correctly followed. </t>
   </si>
+  <si>
+    <t>Select/Deselect All</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1141,11 +1144,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="15"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="38">
@@ -1571,7 +1569,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1633,13 +1631,6 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="37" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1658,6 +1649,16 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="14" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="8" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="8"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Dekorfärg1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1811,6 +1812,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <strike/>
         <color theme="0" tint="-0.499984740745262"/>
       </font>
@@ -1880,16 +1891,6 @@
       <fill>
         <patternFill>
           <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2099,15 +2100,15 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp142.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$F$7" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$7" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp143.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$F$8" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$8" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp144.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$F$9" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$9" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp145.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2328,6 +2329,10 @@
 
 <file path=xl/ctrlProps/ctrlProp194.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$76" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp195.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$3" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -12152,9 +12157,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>390769</xdr:colOff>
+          <xdr:colOff>393700</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>12153</xdr:rowOff>
+          <xdr:rowOff>12700</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -12164,7 +12169,7 @@
                   <a14:compatExt spid="_x0000_s3308"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3060744-8F8F-BA8A-0678-943F58B08E0E}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000EC0C0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -12221,7 +12226,7 @@
           <xdr:col>4</xdr:col>
           <xdr:colOff>393700</xdr:colOff>
           <xdr:row>8</xdr:row>
-          <xdr:rowOff>12699</xdr:rowOff>
+          <xdr:rowOff>12700</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -12231,7 +12236,7 @@
                   <a14:compatExt spid="_x0000_s3309"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9CA45A59-1714-7500-D382-A1C0538E7E9F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000ED0C0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -12288,7 +12293,7 @@
           <xdr:col>4</xdr:col>
           <xdr:colOff>393700</xdr:colOff>
           <xdr:row>9</xdr:row>
-          <xdr:rowOff>12701</xdr:rowOff>
+          <xdr:rowOff>12700</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -12298,7 +12303,7 @@
                   <a14:compatExt spid="_x0000_s3311"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{33B08AA5-8D76-6471-88E0-2EF8B279DC6F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000EF0C0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -12355,7 +12360,7 @@
           <xdr:col>4</xdr:col>
           <xdr:colOff>393700</xdr:colOff>
           <xdr:row>10</xdr:row>
-          <xdr:rowOff>12699</xdr:rowOff>
+          <xdr:rowOff>12700</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -12365,7 +12370,7 @@
                   <a14:compatExt spid="_x0000_s3312"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ABF0C766-B343-AA13-F321-283DA91D9E79}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000F00C0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -12422,7 +12427,7 @@
           <xdr:col>4</xdr:col>
           <xdr:colOff>393700</xdr:colOff>
           <xdr:row>11</xdr:row>
-          <xdr:rowOff>12701</xdr:rowOff>
+          <xdr:rowOff>12700</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -12432,7 +12437,7 @@
                   <a14:compatExt spid="_x0000_s3313"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B3DF4D94-E03A-3844-B1FF-2853591E2299}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000F10C0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -12489,7 +12494,7 @@
           <xdr:col>4</xdr:col>
           <xdr:colOff>393700</xdr:colOff>
           <xdr:row>12</xdr:row>
-          <xdr:rowOff>12699</xdr:rowOff>
+          <xdr:rowOff>12700</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -12499,7 +12504,7 @@
                   <a14:compatExt spid="_x0000_s3314"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{910C51FB-52DF-94AC-5BE7-0798420661B4}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000F20C0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -12556,7 +12561,7 @@
           <xdr:col>4</xdr:col>
           <xdr:colOff>393700</xdr:colOff>
           <xdr:row>13</xdr:row>
-          <xdr:rowOff>12701</xdr:rowOff>
+          <xdr:rowOff>12700</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -12566,7 +12571,7 @@
                   <a14:compatExt spid="_x0000_s3315"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{83D262E2-43BD-0344-2EE2-2F63996136C3}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000F30C0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -12633,7 +12638,7 @@
                   <a14:compatExt spid="_x0000_s3316"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A85C76D0-7334-2A65-A0BA-E85A7EB4F9D2}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000F40C0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -12690,7 +12695,7 @@
           <xdr:col>4</xdr:col>
           <xdr:colOff>393700</xdr:colOff>
           <xdr:row>17</xdr:row>
-          <xdr:rowOff>12699</xdr:rowOff>
+          <xdr:rowOff>12700</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -12700,7 +12705,7 @@
                   <a14:compatExt spid="_x0000_s3321"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{006A3F0F-5F1C-7404-28B4-373F0801C12C}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000F90C0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -12757,7 +12762,7 @@
           <xdr:col>4</xdr:col>
           <xdr:colOff>393700</xdr:colOff>
           <xdr:row>18</xdr:row>
-          <xdr:rowOff>12701</xdr:rowOff>
+          <xdr:rowOff>12700</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -12767,7 +12772,7 @@
                   <a14:compatExt spid="_x0000_s3322"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4DAFAC66-A303-B8B6-A60F-97203B37F0E7}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000FA0C0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -12824,7 +12829,7 @@
           <xdr:col>4</xdr:col>
           <xdr:colOff>393700</xdr:colOff>
           <xdr:row>19</xdr:row>
-          <xdr:rowOff>12699</xdr:rowOff>
+          <xdr:rowOff>12700</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -12834,7 +12839,7 @@
                   <a14:compatExt spid="_x0000_s3323"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{103FECE6-B6DD-3F50-A04C-CAEE9A37F7C2}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000FB0C0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -12891,7 +12896,7 @@
           <xdr:col>4</xdr:col>
           <xdr:colOff>393700</xdr:colOff>
           <xdr:row>20</xdr:row>
-          <xdr:rowOff>12701</xdr:rowOff>
+          <xdr:rowOff>12700</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -12901,7 +12906,7 @@
                   <a14:compatExt spid="_x0000_s3324"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E58F52B8-A7EB-2886-83A8-72548035F5AC}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000FC0C0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -12958,7 +12963,7 @@
           <xdr:col>4</xdr:col>
           <xdr:colOff>393700</xdr:colOff>
           <xdr:row>21</xdr:row>
-          <xdr:rowOff>12699</xdr:rowOff>
+          <xdr:rowOff>12700</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -12968,7 +12973,7 @@
                   <a14:compatExt spid="_x0000_s3325"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A28BBFDA-B58C-4D88-DB85-4735664ED57F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000FD0C0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -13025,7 +13030,7 @@
           <xdr:col>4</xdr:col>
           <xdr:colOff>393700</xdr:colOff>
           <xdr:row>22</xdr:row>
-          <xdr:rowOff>12701</xdr:rowOff>
+          <xdr:rowOff>12700</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -13035,7 +13040,7 @@
                   <a14:compatExt spid="_x0000_s3326"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A096B925-E9C4-526A-CAAA-A88D3E960603}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000FE0C0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -13102,7 +13107,7 @@
                   <a14:compatExt spid="_x0000_s3327"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{85FFECEA-950A-9794-60A2-DE52065A6D6D}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000FF0C0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -13158,8 +13163,8 @@
         <xdr:to>
           <xdr:col>4</xdr:col>
           <xdr:colOff>393700</xdr:colOff>
-          <xdr:row>26</xdr:row>
-          <xdr:rowOff>200526</xdr:rowOff>
+          <xdr:row>27</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -13169,7 +13174,7 @@
                   <a14:compatExt spid="_x0000_s3328"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CF1B086-DBEE-2763-DF50-EF92D7E737BC}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000000D0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -13226,7 +13231,7 @@
           <xdr:col>4</xdr:col>
           <xdr:colOff>393700</xdr:colOff>
           <xdr:row>28</xdr:row>
-          <xdr:rowOff>1</xdr:rowOff>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -13236,7 +13241,7 @@
                   <a14:compatExt spid="_x0000_s3329"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{71B315D2-DC11-33E5-75FE-E781D21443B4}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000010D0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -13303,7 +13308,7 @@
                   <a14:compatExt spid="_x0000_s3330"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{35862770-7002-16A5-F583-B334664FB055}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000020D0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -13360,7 +13365,7 @@
           <xdr:col>4</xdr:col>
           <xdr:colOff>393700</xdr:colOff>
           <xdr:row>32</xdr:row>
-          <xdr:rowOff>1</xdr:rowOff>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -13370,7 +13375,7 @@
                   <a14:compatExt spid="_x0000_s3331"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A09B4FA-AF9E-C5FC-5449-B4E19BFFD4C0}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000030D0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -13437,7 +13442,7 @@
                   <a14:compatExt spid="_x0000_s3332"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E6E1A3B-B9A6-FF38-31D3-32F7E59189B1}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000040D0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -13504,7 +13509,7 @@
                   <a14:compatExt spid="_x0000_s3333"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FAE5E17B-41E9-523D-F7C7-9189A55D045D}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000050D0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -13561,7 +13566,7 @@
           <xdr:col>4</xdr:col>
           <xdr:colOff>393700</xdr:colOff>
           <xdr:row>37</xdr:row>
-          <xdr:rowOff>1</xdr:rowOff>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -13571,7 +13576,7 @@
                   <a14:compatExt spid="_x0000_s3334"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F9F1E993-5B2C-8A2D-451D-09761CF2BDF3}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000060D0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -13638,7 +13643,7 @@
                   <a14:compatExt spid="_x0000_s3335"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{216357F9-32A6-1C64-5643-6B5FD93C5528}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000070D0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -13705,7 +13710,7 @@
                   <a14:compatExt spid="_x0000_s3336"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50C9CA8A-7884-DFA2-31EC-2EF3AACEFFBD}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000080D0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -13772,7 +13777,7 @@
                   <a14:compatExt spid="_x0000_s3337"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F24B7B9C-07DD-1893-FC4E-DFB41650FA3F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000090D0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -13839,7 +13844,7 @@
                   <a14:compatExt spid="_x0000_s3338"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DFB315DC-48D4-E7D9-EADD-7CAF0A0B9DE9}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000A0D0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -13895,8 +13900,8 @@
         <xdr:to>
           <xdr:col>4</xdr:col>
           <xdr:colOff>393700</xdr:colOff>
-          <xdr:row>43</xdr:row>
-          <xdr:rowOff>200526</xdr:rowOff>
+          <xdr:row>44</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -13906,7 +13911,7 @@
                   <a14:compatExt spid="_x0000_s3339"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F852120C-A3CC-1673-FC02-63E189AE2658}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000B0D0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -13963,7 +13968,7 @@
           <xdr:col>4</xdr:col>
           <xdr:colOff>393700</xdr:colOff>
           <xdr:row>45</xdr:row>
-          <xdr:rowOff>1</xdr:rowOff>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -13973,7 +13978,7 @@
                   <a14:compatExt spid="_x0000_s3340"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF14C636-2EB7-3AEE-97D5-CA6B693A6A68}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000C0D0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -14040,7 +14045,7 @@
                   <a14:compatExt spid="_x0000_s3342"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{736EB423-375F-E0BC-82DD-CAC461B2923F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000E0D0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -14096,8 +14101,8 @@
         <xdr:to>
           <xdr:col>4</xdr:col>
           <xdr:colOff>393700</xdr:colOff>
-          <xdr:row>46</xdr:row>
-          <xdr:rowOff>200526</xdr:rowOff>
+          <xdr:row>47</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -14107,7 +14112,7 @@
                   <a14:compatExt spid="_x0000_s3343"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{55D4623D-6ECA-6401-D960-E74C9DE0C000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000F0D0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -14164,7 +14169,7 @@
           <xdr:col>4</xdr:col>
           <xdr:colOff>393700</xdr:colOff>
           <xdr:row>48</xdr:row>
-          <xdr:rowOff>1</xdr:rowOff>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -14174,7 +14179,7 @@
                   <a14:compatExt spid="_x0000_s3344"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2391A691-ECF4-7A86-50D9-9A4197C28547}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000100D0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -14241,7 +14246,7 @@
                   <a14:compatExt spid="_x0000_s3345"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7F5B5449-48E0-534E-4AFE-062F9992ADB5}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000110D0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -14308,7 +14313,7 @@
                   <a14:compatExt spid="_x0000_s3346"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD4BECC3-FB89-199A-25B2-6060632E85F9}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000120D0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -14364,8 +14369,8 @@
         <xdr:to>
           <xdr:col>4</xdr:col>
           <xdr:colOff>393700</xdr:colOff>
-          <xdr:row>52</xdr:row>
-          <xdr:rowOff>200526</xdr:rowOff>
+          <xdr:row>53</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -14375,7 +14380,7 @@
                   <a14:compatExt spid="_x0000_s3347"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA0C456B-DFC6-F349-13C1-F44937622E8A}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000130D0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -14432,7 +14437,7 @@
           <xdr:col>4</xdr:col>
           <xdr:colOff>393700</xdr:colOff>
           <xdr:row>54</xdr:row>
-          <xdr:rowOff>1</xdr:rowOff>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -14442,7 +14447,7 @@
                   <a14:compatExt spid="_x0000_s3348"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7BEC7E02-54EF-EDCB-5AED-351709135ABC}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000140D0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -14509,7 +14514,7 @@
                   <a14:compatExt spid="_x0000_s3349"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8462B498-78A8-77EB-D391-7D778826B136}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000150D0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -14565,8 +14570,8 @@
         <xdr:to>
           <xdr:col>4</xdr:col>
           <xdr:colOff>393700</xdr:colOff>
-          <xdr:row>55</xdr:row>
-          <xdr:rowOff>200526</xdr:rowOff>
+          <xdr:row>56</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -14576,7 +14581,7 @@
                   <a14:compatExt spid="_x0000_s3351"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8FF4CA1B-249C-B0C9-E34A-DF1577A5E55A}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000170D0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -14633,7 +14638,7 @@
           <xdr:col>4</xdr:col>
           <xdr:colOff>393700</xdr:colOff>
           <xdr:row>57</xdr:row>
-          <xdr:rowOff>1</xdr:rowOff>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -14643,7 +14648,7 @@
                   <a14:compatExt spid="_x0000_s3352"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{451C049E-4599-E7F5-63D6-95097F83926D}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000180D0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -14710,7 +14715,7 @@
                   <a14:compatExt spid="_x0000_s3353"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C56B7CCD-1285-C3C6-BB76-C91E278AEED4}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000190D0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -14766,8 +14771,8 @@
         <xdr:to>
           <xdr:col>4</xdr:col>
           <xdr:colOff>393700</xdr:colOff>
-          <xdr:row>58</xdr:row>
-          <xdr:rowOff>200526</xdr:rowOff>
+          <xdr:row>59</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -14777,7 +14782,7 @@
                   <a14:compatExt spid="_x0000_s3354"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C356A095-D899-DF3A-CE0F-3DDBCA5183A2}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00001A0D0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -14834,7 +14839,7 @@
           <xdr:col>4</xdr:col>
           <xdr:colOff>393700</xdr:colOff>
           <xdr:row>60</xdr:row>
-          <xdr:rowOff>1</xdr:rowOff>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -14844,7 +14849,7 @@
                   <a14:compatExt spid="_x0000_s3355"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4CA85DFE-129F-2E78-2F3E-45ABD19F6E9A}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00001B0D0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -14911,7 +14916,7 @@
                   <a14:compatExt spid="_x0000_s3356"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E0977F5-7530-2DA0-7EEC-B198ED5740F6}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00001C0D0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -14957,14 +14962,19 @@
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>63</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="393700" cy="200527"/>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>393700</xdr:colOff>
+          <xdr:row>64</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3357" name="Check Box 285" hidden="1">
@@ -14973,7 +14983,7 @@
                   <a14:compatExt spid="_x0000_s3357"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D457E8EB-0ED3-8844-91BF-2387F96F8111}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00001D0D0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -15013,20 +15023,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>64</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="393700" cy="200526"/>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>393700</xdr:colOff>
+          <xdr:row>65</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3358" name="Check Box 286" hidden="1">
@@ -15035,7 +15050,7 @@
                   <a14:compatExt spid="_x0000_s3358"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9BC9FA92-293D-A04C-83E4-DF45D6933EC0}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00001E0D0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -15075,20 +15090,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>65</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="393700" cy="200526"/>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>393700</xdr:colOff>
+          <xdr:row>66</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3359" name="Check Box 287" hidden="1">
@@ -15097,7 +15117,7 @@
                   <a14:compatExt spid="_x0000_s3359"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9CA1EC24-38EA-CF40-B822-05D85CD2FE34}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00001F0D0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -15137,20 +15157,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>66</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="393700" cy="200527"/>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>393700</xdr:colOff>
+          <xdr:row>67</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3360" name="Check Box 288" hidden="1">
@@ -15159,7 +15184,7 @@
                   <a14:compatExt spid="_x0000_s3360"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{93250C02-FB57-A04B-8B13-F710C72BF1FF}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000200D0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -15199,20 +15224,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>67</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="393700" cy="200526"/>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>393700</xdr:colOff>
+          <xdr:row>68</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3361" name="Check Box 289" hidden="1">
@@ -15221,7 +15251,7 @@
                   <a14:compatExt spid="_x0000_s3361"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{107D6131-F52C-BE40-BA8F-6AF69ED6E561}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000210D0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -15261,7 +15291,7 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
@@ -15278,7 +15308,7 @@
           <xdr:col>4</xdr:col>
           <xdr:colOff>393700</xdr:colOff>
           <xdr:row>69</xdr:row>
-          <xdr:rowOff>1</xdr:rowOff>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -15288,7 +15318,7 @@
                   <a14:compatExt spid="_x0000_s3362"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F9A954F5-675F-FDFC-76F0-E8C8E38E12C3}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000220D0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -15334,14 +15364,19 @@
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>71</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="393700" cy="200527"/>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>393700</xdr:colOff>
+          <xdr:row>72</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3363" name="Check Box 291" hidden="1">
@@ -15350,7 +15385,7 @@
                   <a14:compatExt spid="_x0000_s3363"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED36E739-F1E0-184C-9185-00C6FE1F513B}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000230D0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -15390,20 +15425,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>72</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="393700" cy="200526"/>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>393700</xdr:colOff>
+          <xdr:row>73</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3364" name="Check Box 292" hidden="1">
@@ -15412,7 +15452,7 @@
                   <a14:compatExt spid="_x0000_s3364"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{03441DF3-DDA4-7844-B533-AD85537DA315}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000240D0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -15452,20 +15492,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>73</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="393700" cy="200526"/>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>393700</xdr:colOff>
+          <xdr:row>74</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3365" name="Check Box 293" hidden="1">
@@ -15474,7 +15519,7 @@
                   <a14:compatExt spid="_x0000_s3365"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C0184DB-6F03-AA47-B5C9-FA01CEF333EA}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000250D0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -15514,20 +15559,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>74</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="393700" cy="200527"/>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>393700</xdr:colOff>
+          <xdr:row>75</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3366" name="Check Box 294" hidden="1">
@@ -15536,7 +15586,7 @@
                   <a14:compatExt spid="_x0000_s3366"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB8C01A4-D30E-174E-A245-BCF2AB9FA0C8}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000260D0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -15576,20 +15626,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>75</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="393700" cy="200526"/>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>393700</xdr:colOff>
+          <xdr:row>76</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3367" name="Check Box 295" hidden="1">
@@ -15598,7 +15653,7 @@
                   <a14:compatExt spid="_x0000_s3367"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C8B610A7-DE60-0E40-83D9-CAE60A22E38D}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000270D0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -15638,7 +15693,74 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>393700</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>12700</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3369" name="Check Box 297" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s3369"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BA9B9283-2E33-ED97-7A8C-5C6B961EA8E4}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
@@ -15942,6 +16064,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Blad1"/>
   <dimension ref="A1:H215"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
@@ -20057,6 +20180,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr codeName="Blad2"/>
   <dimension ref="A4:H22"/>
   <sheetViews>
     <sheetView zoomScale="173" workbookViewId="0">
@@ -20713,6 +20837,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5D8C981-CB5D-4B8E-AE76-2A5C315E2101}">
+  <sheetPr codeName="Blad3"/>
   <dimension ref="A2:D13"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
@@ -20830,10 +20955,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55A227F7-73A5-48FB-8BA8-6FE3DE29DA5B}">
+  <sheetPr codeName="Blad4"/>
   <dimension ref="A2:G91"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="133" zoomScaleNormal="358" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -20846,8 +20972,17 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="48" x14ac:dyDescent="0.2">
-      <c r="G2" s="41" t="s">
+      <c r="G2" s="38" t="s">
         <v>258</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D3" s="41" t="s">
+        <v>259</v>
+      </c>
+      <c r="E3" s="42"/>
+      <c r="F3" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -20887,12 +21022,12 @@
       <c r="C7" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="D7" s="38" t="s">
+      <c r="D7" s="35" t="s">
         <v>120</v>
       </c>
-      <c r="E7" s="37"/>
+      <c r="E7" s="34"/>
       <c r="F7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -20902,11 +21037,11 @@
       <c r="C8" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="D8" s="38" t="s">
+      <c r="D8" s="35" t="s">
         <v>121</v>
       </c>
       <c r="F8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -20916,11 +21051,11 @@
       <c r="C9" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="D9" s="38" t="s">
+      <c r="D9" s="35" t="s">
         <v>122</v>
       </c>
       <c r="F9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -20930,7 +21065,7 @@
       <c r="C10" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="38" t="s">
+      <c r="D10" s="35" t="s">
         <v>148</v>
       </c>
       <c r="F10" t="b">
@@ -20944,7 +21079,7 @@
       <c r="C11" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="D11" s="38" t="s">
+      <c r="D11" s="35" t="s">
         <v>205</v>
       </c>
       <c r="F11" t="b">
@@ -20958,7 +21093,7 @@
       <c r="C12" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="D12" s="38" t="s">
+      <c r="D12" s="35" t="s">
         <v>123</v>
       </c>
       <c r="F12" t="b">
@@ -20972,7 +21107,7 @@
       <c r="C13" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="D13" s="38" t="s">
+      <c r="D13" s="35" t="s">
         <v>124</v>
       </c>
       <c r="F13" t="b">
@@ -20984,7 +21119,7 @@
       <c r="C14" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="D14" s="38" t="s">
+      <c r="D14" s="35" t="s">
         <v>206</v>
       </c>
       <c r="F14" t="b">
@@ -21007,7 +21142,7 @@
       <c r="C17" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="D17" s="35" t="s">
+      <c r="D17" s="32" t="s">
         <v>127</v>
       </c>
       <c r="F17" t="b">
@@ -21018,7 +21153,7 @@
       <c r="C18" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="D18" s="35" t="s">
+      <c r="D18" s="32" t="s">
         <v>152</v>
       </c>
       <c r="F18" t="b">
@@ -21029,7 +21164,7 @@
       <c r="C19" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="D19" s="36" t="s">
+      <c r="D19" s="33" t="s">
         <v>129</v>
       </c>
       <c r="F19" t="b">
@@ -21040,7 +21175,7 @@
       <c r="C20" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="D20" s="36" t="s">
+      <c r="D20" s="33" t="s">
         <v>130</v>
       </c>
       <c r="F20" t="b">
@@ -21051,7 +21186,7 @@
       <c r="C21" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="D21" s="35" t="s">
+      <c r="D21" s="32" t="s">
         <v>128</v>
       </c>
       <c r="F21" t="b">
@@ -21062,7 +21197,7 @@
       <c r="C22" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="D22" s="35" t="s">
+      <c r="D22" s="32" t="s">
         <v>131</v>
       </c>
       <c r="F22" t="b">
@@ -21087,7 +21222,7 @@
       <c r="C26" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="D26" s="34" t="s">
+      <c r="D26" s="31" t="s">
         <v>24</v>
       </c>
       <c r="F26" t="b">
@@ -21098,7 +21233,7 @@
       <c r="C27" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="D27" s="34" t="s">
+      <c r="D27" s="31" t="s">
         <v>25</v>
       </c>
       <c r="F27" t="b">
@@ -21109,7 +21244,7 @@
       <c r="C28" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="D28" s="34" t="s">
+      <c r="D28" s="31" t="s">
         <v>26</v>
       </c>
       <c r="F28" t="b">
@@ -21131,7 +21266,7 @@
       <c r="C31" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="D31" s="39" t="s">
+      <c r="D31" s="36" t="s">
         <v>28</v>
       </c>
       <c r="F31" t="b">
@@ -21142,7 +21277,7 @@
       <c r="C32" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="D32" s="34" t="s">
+      <c r="D32" s="31" t="s">
         <v>29</v>
       </c>
       <c r="F32" t="b">
@@ -21153,7 +21288,7 @@
       <c r="C33" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="D33" s="34" t="s">
+      <c r="D33" s="31" t="s">
         <v>30</v>
       </c>
       <c r="F33" t="b">
@@ -21175,7 +21310,7 @@
       <c r="C36" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="D36" s="34" t="s">
+      <c r="D36" s="31" t="s">
         <v>32</v>
       </c>
       <c r="F36" t="b">
@@ -21186,7 +21321,7 @@
       <c r="C37" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="D37" s="34" t="s">
+      <c r="D37" s="31" t="s">
         <v>33</v>
       </c>
       <c r="F37" t="b">
@@ -21197,7 +21332,7 @@
       <c r="C38" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="D38" s="34" t="s">
+      <c r="D38" s="31" t="s">
         <v>158</v>
       </c>
       <c r="F38" t="b">
@@ -21208,7 +21343,7 @@
       <c r="C39" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="D39" s="34" t="s">
+      <c r="D39" s="31" t="s">
         <v>34</v>
       </c>
       <c r="F39" t="b">
@@ -21219,7 +21354,7 @@
       <c r="C40" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="D40" s="34" t="s">
+      <c r="D40" s="31" t="s">
         <v>98</v>
       </c>
       <c r="F40" t="b">
@@ -21238,7 +21373,7 @@
       <c r="C43" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D43" s="34" t="s">
+      <c r="D43" s="31" t="s">
         <v>64</v>
       </c>
       <c r="F43" t="b">
@@ -21249,7 +21384,7 @@
       <c r="C44" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D44" s="34" t="s">
+      <c r="D44" s="31" t="s">
         <v>177</v>
       </c>
       <c r="F44" t="b">
@@ -21260,7 +21395,7 @@
       <c r="C45" s="10" t="s">
         <v>204</v>
       </c>
-      <c r="D45" s="34" t="s">
+      <c r="D45" s="31" t="s">
         <v>176</v>
       </c>
       <c r="F45" t="b">
@@ -21271,7 +21406,7 @@
       <c r="C46" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="D46" s="34" t="s">
+      <c r="D46" s="31" t="s">
         <v>178</v>
       </c>
       <c r="F46" t="b">
@@ -21282,7 +21417,7 @@
       <c r="C47" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D47" s="34" t="s">
+      <c r="D47" s="31" t="s">
         <v>179</v>
       </c>
       <c r="F47" t="b">
@@ -21293,7 +21428,7 @@
       <c r="C48" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="D48" s="34" t="s">
+      <c r="D48" s="31" t="s">
         <v>176</v>
       </c>
       <c r="F48" t="b">
@@ -21304,7 +21439,7 @@
       <c r="C49" s="10" t="s">
         <v>204</v>
       </c>
-      <c r="D49" s="34" t="s">
+      <c r="D49" s="31" t="s">
         <v>180</v>
       </c>
       <c r="F49" t="b">
@@ -21326,7 +21461,7 @@
       <c r="C52" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D52" s="40" t="s">
+      <c r="D52" s="37" t="s">
         <v>213</v>
       </c>
       <c r="F52" t="b">
@@ -21337,7 +21472,7 @@
       <c r="C53" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="D53" s="40" t="s">
+      <c r="D53" s="37" t="s">
         <v>214</v>
       </c>
       <c r="F53" t="b">
@@ -21348,7 +21483,7 @@
       <c r="C54" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="D54" s="40" t="s">
+      <c r="D54" s="37" t="s">
         <v>215</v>
       </c>
       <c r="F54" t="b">
@@ -21359,7 +21494,7 @@
       <c r="C55" s="10" t="s">
         <v>181</v>
       </c>
-      <c r="D55" s="40" t="s">
+      <c r="D55" s="37" t="s">
         <v>216</v>
       </c>
       <c r="F55" t="b">
@@ -21370,7 +21505,7 @@
       <c r="C56" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="D56" s="40" t="s">
+      <c r="D56" s="37" t="s">
         <v>210</v>
       </c>
       <c r="F56" t="b">
@@ -21381,7 +21516,7 @@
       <c r="C57" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D57" s="40" t="s">
+      <c r="D57" s="37" t="s">
         <v>217</v>
       </c>
       <c r="F57" t="b">
@@ -21392,7 +21527,7 @@
       <c r="C58" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="D58" s="40" t="s">
+      <c r="D58" s="37" t="s">
         <v>214</v>
       </c>
       <c r="F58" t="b">
@@ -21403,7 +21538,7 @@
       <c r="C59" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="D59" s="40" t="s">
+      <c r="D59" s="37" t="s">
         <v>218</v>
       </c>
       <c r="F59" t="b">
@@ -21414,7 +21549,7 @@
       <c r="C60" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="D60" s="40" t="s">
+      <c r="D60" s="37" t="s">
         <v>216</v>
       </c>
       <c r="F60" t="b">
@@ -21425,7 +21560,7 @@
       <c r="C61" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="D61" s="40" t="s">
+      <c r="D61" s="37" t="s">
         <v>212</v>
       </c>
       <c r="F61" t="b">
@@ -21444,7 +21579,7 @@
       <c r="C64" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D64" s="40" t="s">
+      <c r="D64" s="37" t="s">
         <v>208</v>
       </c>
       <c r="F64" t="b">
@@ -21455,7 +21590,7 @@
       <c r="C65" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="D65" s="40" t="s">
+      <c r="D65" s="37" t="s">
         <v>209</v>
       </c>
       <c r="F65" t="b">
@@ -21466,7 +21601,7 @@
       <c r="C66" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="D66" s="40" t="s">
+      <c r="D66" s="37" t="s">
         <v>210</v>
       </c>
       <c r="F66" t="b">
@@ -21477,7 +21612,7 @@
       <c r="C67" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D67" s="40" t="s">
+      <c r="D67" s="37" t="s">
         <v>211</v>
       </c>
       <c r="F67" t="b">
@@ -21488,7 +21623,7 @@
       <c r="C68" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="D68" s="40" t="s">
+      <c r="D68" s="37" t="s">
         <v>209</v>
       </c>
       <c r="F68" t="b">
@@ -21499,7 +21634,7 @@
       <c r="C69" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="D69" s="40" t="s">
+      <c r="D69" s="37" t="s">
         <v>212</v>
       </c>
       <c r="F69" t="b">
@@ -21516,7 +21651,7 @@
       <c r="C72" s="10" t="s">
         <v>181</v>
       </c>
-      <c r="D72" s="40" t="s">
+      <c r="D72" s="37" t="s">
         <v>219</v>
       </c>
       <c r="F72" t="b">
@@ -21527,7 +21662,7 @@
       <c r="C73" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D73" s="40" t="s">
+      <c r="D73" s="37" t="s">
         <v>220</v>
       </c>
       <c r="F73" t="b">
@@ -21538,7 +21673,7 @@
       <c r="C74" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="D74" s="40" t="s">
+      <c r="D74" s="37" t="s">
         <v>221</v>
       </c>
       <c r="F74" t="b">
@@ -21549,7 +21684,7 @@
       <c r="C75" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D75" s="40" t="s">
+      <c r="D75" s="37" t="s">
         <v>222</v>
       </c>
       <c r="F75" t="b">
@@ -21560,7 +21695,7 @@
       <c r="C76" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="D76" s="40" t="s">
+      <c r="D76" s="37" t="s">
         <v>223</v>
       </c>
       <c r="F76" t="b">
@@ -21572,23 +21707,17 @@
         <v>233</v>
       </c>
     </row>
-    <row r="79" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C79" s="31"/>
-    </row>
     <row r="80" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C80" s="32" t="s">
+      <c r="C80" s="39" t="s">
         <v>255</v>
       </c>
-      <c r="D80" s="33"/>
-    </row>
-    <row r="81" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C81" s="31"/>
+      <c r="D80" s="40"/>
     </row>
     <row r="82" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C82" s="32" t="s">
+      <c r="C82" s="39" t="s">
         <v>256</v>
       </c>
-      <c r="D82" s="33"/>
+      <c r="D82" s="40"/>
     </row>
     <row r="85" spans="3:4" ht="16" x14ac:dyDescent="0.2">
       <c r="D85" s="30" t="s">
@@ -21632,35 +21761,35 @@
   </mergeCells>
   <phoneticPr fontId="20" type="noConversion"/>
   <conditionalFormatting sqref="D7:D14">
-    <cfRule type="expression" dxfId="17" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="22">
+      <formula>$F7</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="16" priority="18" stopIfTrue="1">
       <formula>AND($F7=FALSE,$F6&lt;&gt;FALSE)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="16" priority="22">
-      <formula>$F7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D17:D22">
-    <cfRule type="expression" dxfId="15" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="17">
+      <formula>$F17</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="14" priority="16" stopIfTrue="1">
       <formula>AND($F17=FALSE,$F16&lt;&gt;FALSE)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="14" priority="17">
-      <formula>$F17</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D26:D28">
-    <cfRule type="expression" dxfId="13" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="14">
+      <formula>$F26</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="12" priority="13" stopIfTrue="1">
       <formula>AND($F26=FALSE,$F25&lt;&gt;FALSE)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="12" priority="14">
-      <formula>$F26</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D31:D33">
-    <cfRule type="expression" dxfId="11" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="12">
+      <formula>$F31</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="11" stopIfTrue="1">
       <formula>AND($F31=FALSE,$F30&lt;&gt;FALSE)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="10" priority="12">
-      <formula>$F31</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D36:D40">
@@ -22876,6 +23005,28 @@
             </control>
           </mc:Choice>
         </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="3369" r:id="rId57" name="Check Box 297">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" macro="[0]!AllCheckBoxes">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>2</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>393700</xdr:colOff>
+                    <xdr:row>3</xdr:row>
+                    <xdr:rowOff>12700</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
       </controls>
     </mc:Choice>
   </mc:AlternateContent>
@@ -22884,6 +23035,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5439C230-43A8-4EDF-B554-2E24F8DC7117}">
+  <sheetPr codeName="Blad5"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -22898,6 +23050,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26EB917C-8484-4DF8-A5FA-675B4F617B65}">
+  <sheetPr codeName="Blad6"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Cleaned up the roles page a bit
</commit_message>
<xml_diff>
--- a/mainProcedure.xlsx
+++ b/mainProcedure.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexandragustafsson/Documents/TCRYA-civ.ing/RAVEN - som inte finns på teams/RavenProcedure/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55B3E587-7FD1-1044-A319-EAB1726BEE66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB280F9C-2DD7-5042-8899-86CCA49FD63A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mainProcedure" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="259">
   <si>
     <t>Version</t>
   </si>
@@ -401,9 +401,6 @@
     <t>Supervisor</t>
   </si>
   <si>
-    <t>Engine setup</t>
-  </si>
-  <si>
     <t>Ganesh</t>
   </si>
   <si>
@@ -413,9 +410,6 @@
     <t>Ivar</t>
   </si>
   <si>
-    <t>Someone</t>
-  </si>
-  <si>
     <t>Check that umbilical is connected to controlbox</t>
   </si>
   <si>
@@ -512,12 +506,6 @@
     <t>Heating of bottle</t>
   </si>
   <si>
-    <t>Person 1</t>
-  </si>
-  <si>
-    <t>Person 2</t>
-  </si>
-  <si>
     <t>Pre Procedures</t>
   </si>
   <si>
@@ -530,16 +518,10 @@
     <t>Action</t>
   </si>
   <si>
-    <t>MG</t>
-  </si>
-  <si>
     <t>Lukas</t>
   </si>
   <si>
     <t>Alexandra</t>
-  </si>
-  <si>
-    <t>EL</t>
   </si>
   <si>
     <t>EL1</t>
@@ -944,12 +926,48 @@
   <si>
     <t>Pre procedure?</t>
   </si>
+  <si>
+    <t>SUP</t>
+  </si>
+  <si>
+    <t>ES1</t>
+  </si>
+  <si>
+    <t>ES2</t>
+  </si>
+  <si>
+    <t>Electronics 1</t>
+  </si>
+  <si>
+    <t>Electronics 2</t>
+  </si>
+  <si>
+    <t>Engine setup 1</t>
+  </si>
+  <si>
+    <t>Engine setup 2</t>
+  </si>
+  <si>
+    <t>Electronics Team</t>
+  </si>
+  <si>
+    <t>Rocket Motor - RM</t>
+  </si>
+  <si>
+    <t>People</t>
+  </si>
+  <si>
+    <t>Attendance</t>
+  </si>
+  <si>
+    <t>Roles</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1122,6 +1140,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="38">
@@ -1547,7 +1570,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1645,6 +1668,8 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Dekorfärg1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1690,7 +1715,7 @@
     <cellStyle name="Utdata" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Varningstext" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="26">
+  <dxfs count="30">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1713,12 +1738,21 @@
     </dxf>
     <dxf>
       <font>
-        <strike/>
-        <color theme="0" tint="-0.499984740745262"/>
+        <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1772,6 +1806,37 @@
       <fill>
         <patternFill>
           <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1986,43 +2051,43 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp100.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$56" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$45" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp101.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$57" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$46" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp102.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$58" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$47" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp103.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$59" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$48" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp104.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$60" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$49" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp105.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$61" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$52" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp106.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$64" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$53" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp107.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$65" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$54" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp108.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$66" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$55" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp109.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$67" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$56" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp11.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2030,43 +2095,43 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp110.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$68" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$57" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp111.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$69" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$58" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp112.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$72" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$59" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp113.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$73" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$60" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp114.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$74" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$61" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp115.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$75" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$64" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp116.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$76" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$65" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp117.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$3" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$66" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp118.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$80" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$67" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp119.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$81" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$68" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp12.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2074,43 +2139,43 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp120.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$82" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$69" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp121.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$83" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$72" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp122.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$84" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$73" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp123.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$85" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$74" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp124.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$88" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$75" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp125.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$89" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$76" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp126.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$90" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$3" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp127.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$91" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$80" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp128.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$92" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$81" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp129.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$93" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$82" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp13.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2118,43 +2183,43 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp130.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$94" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$83" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp131.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$95" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$84" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp132.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$96" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$85" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp133.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$97" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$88" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp134.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$100" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$89" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp135.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$101" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$90" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp136.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$102" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$91" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp137.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$103" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$92" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp138.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$106" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$93" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp139.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$107" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$94" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp14.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2162,15 +2227,51 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp140.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$108" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$95" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp141.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$3" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$96" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp142.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$97" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp143.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$100" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp144.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$101" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp145.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$102" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp146.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$103" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp147.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$106" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp148.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$107" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp149.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$108" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp15.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp150.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$3" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp16.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2386,27 +2487,27 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp64.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$7" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$5" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp65.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$8" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$3" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp66.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$9" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$8" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp67.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$10" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$9" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp68.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$11" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$10" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp69.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$12" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$11" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp7.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2414,43 +2515,43 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp70.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$13" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$15" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp71.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$14" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$16" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp72.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$17" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$17" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp73.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$18" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$7" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp74.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$19" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$8" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp75.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$20" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$9" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp76.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$21" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$10" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp77.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$22" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$11" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp78.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$26" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$12" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp79.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$27" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$13" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp8.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2458,43 +2559,43 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp80.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$28" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$14" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp81.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$31" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$17" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp82.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$32" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$18" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp83.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$33" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$19" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp84.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$36" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$20" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp85.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$37" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$21" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp86.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$39" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$22" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp87.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$38" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$26" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp88.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$40" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$27" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp89.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$43" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$28" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp9.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2502,43 +2603,43 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp90.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$44" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$31" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp91.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$45" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$32" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp92.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$46" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$33" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp93.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$47" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$36" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp94.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$48" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$37" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp95.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$49" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$39" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp96.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$52" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$38" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp97.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$53" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$40" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp98.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$54" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$43" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp99.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$55" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$44" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6778,6 +6879,614 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>67733</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>186267</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>389467</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>16933</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="6146" name="Check Box 2" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s6146"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6FE9C3F5-9146-85F1-23D4-3F2931B4D786}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>63500</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>393700</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>12700</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="6148" name="Check Box 4" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s6148"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AC8DEF3D-DE6E-0EE5-C3B7-39B29274EB57}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>63500</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>393700</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>12700</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="6149" name="Check Box 5" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s6149"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3AA5C29-E781-2013-60A3-7932EF4E0EEE}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>63500</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>393700</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>12700</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="6151" name="Check Box 7" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s6151"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{90C669B8-3CDC-0454-972F-51CB290B6361}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>63500</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>393700</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>12700</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="6152" name="Check Box 8" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s6152"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D9ADFB2-E82F-C8F4-8046-8F587410E715}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>63500</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>393700</xdr:colOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>12700</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="6153" name="Check Box 9" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s6153"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{64515218-61DA-9753-047D-2C307FBAB504}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>63500</xdr:colOff>
+          <xdr:row>14</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>393700</xdr:colOff>
+          <xdr:row>15</xdr:row>
+          <xdr:rowOff>12700</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="6154" name="Check Box 10" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s6154"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{31A2336C-BFD9-9CB7-8A6F-79E755336DDC}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>63500</xdr:colOff>
+          <xdr:row>15</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>393700</xdr:colOff>
+          <xdr:row>16</xdr:row>
+          <xdr:rowOff>12700</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="6155" name="Check Box 11" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s6155"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F99242DA-5D92-5225-D6CB-F975558BB491}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>63500</xdr:colOff>
+          <xdr:row>16</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>393700</xdr:colOff>
+          <xdr:row>17</xdr:row>
+          <xdr:rowOff>12700</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="6156" name="Check Box 12" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s6156"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B825FBE2-1F91-9FE9-F421-6D9F80BDBDDD}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
           <xdr:col>4</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>6</xdr:row>
@@ -11936,7 +12645,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
@@ -12428,7 +13137,7 @@
     </row>
     <row r="16" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="C16" s="41" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
     </row>
     <row r="17" spans="2:8" ht="16" x14ac:dyDescent="0.2">
@@ -12436,7 +13145,7 @@
         <v>16</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
     </row>
     <row r="18" spans="2:8" ht="16" x14ac:dyDescent="0.2">
@@ -12444,12 +13153,12 @@
         <v>39</v>
       </c>
       <c r="E18" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
     </row>
     <row r="19" spans="2:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C19" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="20" spans="2:8" ht="16" x14ac:dyDescent="0.2">
@@ -12457,7 +13166,7 @@
         <v>9</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.2">
@@ -12501,65 +13210,65 @@
         <v>43</v>
       </c>
       <c r="H27" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
     </row>
     <row r="28" spans="2:8" ht="32" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H28" s="18" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
     </row>
     <row r="29" spans="2:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C29" s="1" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="H29" s="18" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="30" spans="2:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="H30" s="18" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
     </row>
     <row r="31" spans="2:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C31" s="1" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="H31" s="18"/>
     </row>
     <row r="32" spans="2:8" ht="32" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="H32" s="18" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
     </row>
     <row r="33" spans="2:8" ht="32" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H33" s="18" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
     </row>
     <row r="34" spans="2:8" ht="16" x14ac:dyDescent="0.2">
@@ -12567,27 +13276,27 @@
         <v>5</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G34" s="2"/>
       <c r="H34" s="18" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
     </row>
     <row r="35" spans="2:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
+        <v>126</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>128</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="36" spans="2:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
+        <v>127</v>
+      </c>
+      <c r="C36" s="1" t="s">
         <v>129</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.2">
@@ -12644,7 +13353,7 @@
         <v>16</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="46" spans="2:8" ht="16" x14ac:dyDescent="0.2">
@@ -12652,7 +13361,7 @@
         <v>9</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.2">
@@ -12663,7 +13372,7 @@
         <v>49</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -12671,7 +13380,7 @@
         <v>9</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -12679,7 +13388,7 @@
         <v>9</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
@@ -12690,7 +13399,7 @@
         <v>5</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -12698,10 +13407,10 @@
         <v>5</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="E53" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -12709,7 +13418,7 @@
         <v>5</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -12717,7 +13426,7 @@
         <v>5</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
@@ -12736,10 +13445,10 @@
     </row>
     <row r="58" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B58" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -12787,7 +13496,7 @@
         <v>7</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="66" spans="2:3" ht="16" x14ac:dyDescent="0.2">
@@ -12819,7 +13528,7 @@
         <v>7</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="71" spans="2:3" ht="16" x14ac:dyDescent="0.2">
@@ -12827,7 +13536,7 @@
         <v>7</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="73" spans="2:3" ht="16" x14ac:dyDescent="0.2">
@@ -12859,7 +13568,7 @@
         <v>67</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="77" spans="2:3" ht="16" x14ac:dyDescent="0.2">
@@ -12888,7 +13597,7 @@
     </row>
     <row r="81" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="C81" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -12907,20 +13616,20 @@
         <v>16</v>
       </c>
       <c r="C85" s="16" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="C86" s="20" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C87" s="20" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
@@ -12930,47 +13639,47 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C89" s="19" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C90" s="19" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C91" s="19" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C92" s="19" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C93" s="19" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C94" s="19" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C95" s="19" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C96" s="19" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="97" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C97" s="19" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
     </row>
     <row r="98" spans="3:3" x14ac:dyDescent="0.2">
@@ -12980,32 +13689,32 @@
     </row>
     <row r="99" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C99" s="19" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
     </row>
     <row r="100" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C100" s="19" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
     </row>
     <row r="101" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C101" s="19" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
     </row>
     <row r="102" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C102" s="21" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="103" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C103" s="21" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="104" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C104" s="21" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
     </row>
     <row r="127" spans="3:3" x14ac:dyDescent="0.2">
@@ -14704,120 +15413,437 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5D8C981-CB5D-4B8E-AE76-2A5C315E2101}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5D8C981-CB5D-4B8E-AE76-2A5C315E2101}">
   <sheetPr codeName="Blad3"/>
-  <dimension ref="A2:D13"/>
+  <dimension ref="A2:E17"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="14.6640625" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C2" t="s">
-        <v>153</v>
-      </c>
-      <c r="D2" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="45" t="s">
+        <v>258</v>
+      </c>
+      <c r="B2" s="8"/>
+      <c r="C2" s="45" t="s">
+        <v>256</v>
+      </c>
+      <c r="D2" s="45" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="C3" t="s">
-        <v>160</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="C3" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="D3" s="8"/>
+      <c r="E3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="46"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="D5" s="8"/>
+      <c r="E5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="46"/>
+      <c r="B6" s="46"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="46"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="D8" s="8"/>
+      <c r="E8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="8" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C5" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>167</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="B9" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C9" s="8" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>162</v>
-      </c>
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" t="s">
-        <v>119</v>
-      </c>
-      <c r="D7" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
-        <v>77</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="D9" s="8"/>
+      <c r="E9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="D10" s="8"/>
+      <c r="E10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="D11" s="8"/>
+      <c r="E11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="46"/>
+      <c r="B12" s="46"/>
+      <c r="C12" s="46"/>
+      <c r="D12" s="46"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="8" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="8" t="s">
+        <v>247</v>
+      </c>
+      <c r="B15" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C15" s="8" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>159</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="D15" s="8"/>
+      <c r="E15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="8" t="s">
+        <v>248</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="C16" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D16" s="8"/>
+      <c r="E16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="C17" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="D11" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>56</v>
-      </c>
-      <c r="B13" t="s">
-        <v>78</v>
-      </c>
-      <c r="C13" t="s">
-        <v>120</v>
+      <c r="D17" s="8"/>
+      <c r="E17" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A3:C3">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$E3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A5:C5">
+    <cfRule type="expression" dxfId="3" priority="2">
+      <formula>$E5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A8:C11">
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>$E8</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A15:C17">
+    <cfRule type="expression" dxfId="1" priority="4">
+      <formula>$E15</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x14">
+      <controls>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="6146" r:id="rId3" name="Check Box 2">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>63500</xdr:colOff>
+                    <xdr:row>3</xdr:row>
+                    <xdr:rowOff>190500</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>393700</xdr:colOff>
+                    <xdr:row>5</xdr:row>
+                    <xdr:rowOff>12700</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="6148" r:id="rId4" name="Check Box 4">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>63500</xdr:colOff>
+                    <xdr:row>2</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>393700</xdr:colOff>
+                    <xdr:row>3</xdr:row>
+                    <xdr:rowOff>12700</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="6149" r:id="rId5" name="Check Box 5">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>63500</xdr:colOff>
+                    <xdr:row>7</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>393700</xdr:colOff>
+                    <xdr:row>8</xdr:row>
+                    <xdr:rowOff>12700</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="6151" r:id="rId6" name="Check Box 7">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>63500</xdr:colOff>
+                    <xdr:row>8</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>393700</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>12700</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="6152" r:id="rId7" name="Check Box 8">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>63500</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>393700</xdr:colOff>
+                    <xdr:row>10</xdr:row>
+                    <xdr:rowOff>12700</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="6153" r:id="rId8" name="Check Box 9">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>63500</xdr:colOff>
+                    <xdr:row>10</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>393700</xdr:colOff>
+                    <xdr:row>11</xdr:row>
+                    <xdr:rowOff>12700</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="6154" r:id="rId9" name="Check Box 10">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>63500</xdr:colOff>
+                    <xdr:row>14</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>393700</xdr:colOff>
+                    <xdr:row>15</xdr:row>
+                    <xdr:rowOff>12700</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="6155" r:id="rId10" name="Check Box 11">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>63500</xdr:colOff>
+                    <xdr:row>15</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>393700</xdr:colOff>
+                    <xdr:row>16</xdr:row>
+                    <xdr:rowOff>12700</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="6156" r:id="rId11" name="Check Box 12">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>63500</xdr:colOff>
+                    <xdr:row>16</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>393700</xdr:colOff>
+                    <xdr:row>17</xdr:row>
+                    <xdr:rowOff>12700</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+      </controls>
+    </mc:Choice>
+  </mc:AlternateContent>
 </worksheet>
 </file>
 
@@ -14826,7 +15852,7 @@
   <sheetPr codeName="Blad4"/>
   <dimension ref="A2:G123"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="A91" zoomScale="150" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="D100" sqref="D100"/>
     </sheetView>
   </sheetViews>
@@ -14842,12 +15868,12 @@
   <sheetData>
     <row r="2" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="G2" s="36" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D3" s="37" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="E3" s="38"/>
       <c r="F3" t="b">
@@ -14856,16 +15882,16 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B4" s="16" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -14873,7 +15899,7 @@
         <v>14</v>
       </c>
       <c r="F5" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="16" x14ac:dyDescent="0.2">
@@ -14889,7 +15915,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="D7" s="33" t="s">
         <v>95</v>
@@ -14904,7 +15930,7 @@
         <v>2</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="D8" s="33" t="s">
         <v>96</v>
@@ -14918,7 +15944,7 @@
         <v>3</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="D9" s="33" t="s">
         <v>97</v>
@@ -14935,7 +15961,7 @@
         <v>5</v>
       </c>
       <c r="D10" s="33" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F10" t="b">
         <v>0</v>
@@ -14946,10 +15972,10 @@
         <v>5</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="D11" s="33" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="F11" t="b">
         <v>0</v>
@@ -14960,7 +15986,7 @@
         <v>6</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="D12" s="33" t="s">
         <v>98</v>
@@ -14974,7 +16000,7 @@
         <v>7</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="D13" s="33" t="s">
         <v>99</v>
@@ -14986,10 +16012,10 @@
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="15"/>
       <c r="C14" s="8" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="D14" s="33" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="F14" t="b">
         <v>0</v>
@@ -15009,7 +16035,7 @@
     </row>
     <row r="17" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C17" s="8" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="D17" s="30" t="s">
         <v>101</v>
@@ -15020,10 +16046,10 @@
     </row>
     <row r="18" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C18" s="8" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="D18" s="30" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F18" t="b">
         <v>0</v>
@@ -15031,7 +16057,7 @@
     </row>
     <row r="19" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C19" s="8" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="D19" s="31" t="s">
         <v>103</v>
@@ -15042,7 +16068,7 @@
     </row>
     <row r="20" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C20" s="8" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="D20" s="31" t="s">
         <v>104</v>
@@ -15053,7 +16079,7 @@
     </row>
     <row r="21" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C21" s="8" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="D21" s="30" t="s">
         <v>102</v>
@@ -15064,7 +16090,7 @@
     </row>
     <row r="22" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C22" s="8" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="D22" s="30" t="s">
         <v>105</v>
@@ -15089,7 +16115,7 @@
     </row>
     <row r="26" spans="3:6" ht="16" x14ac:dyDescent="0.2">
       <c r="C26" s="8" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="D26" s="29" t="s">
         <v>23</v>
@@ -15100,7 +16126,7 @@
     </row>
     <row r="27" spans="3:6" ht="16" x14ac:dyDescent="0.2">
       <c r="C27" s="8" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="D27" s="29" t="s">
         <v>24</v>
@@ -15111,7 +16137,7 @@
     </row>
     <row r="28" spans="3:6" ht="16" x14ac:dyDescent="0.2">
       <c r="C28" s="8" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="D28" s="29" t="s">
         <v>25</v>
@@ -15133,7 +16159,7 @@
     </row>
     <row r="31" spans="3:6" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C31" s="8" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="D31" s="34" t="s">
         <v>27</v>
@@ -15144,7 +16170,7 @@
     </row>
     <row r="32" spans="3:6" ht="16" x14ac:dyDescent="0.2">
       <c r="C32" s="8" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="D32" s="29" t="s">
         <v>28</v>
@@ -15155,7 +16181,7 @@
     </row>
     <row r="33" spans="3:6" ht="16" x14ac:dyDescent="0.2">
       <c r="C33" s="8" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="D33" s="29" t="s">
         <v>29</v>
@@ -15177,7 +16203,7 @@
     </row>
     <row r="36" spans="3:6" ht="32" x14ac:dyDescent="0.2">
       <c r="C36" s="8" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="D36" s="29" t="s">
         <v>31</v>
@@ -15188,7 +16214,7 @@
     </row>
     <row r="37" spans="3:6" ht="16" x14ac:dyDescent="0.2">
       <c r="C37" s="8" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="D37" s="29" t="s">
         <v>32</v>
@@ -15199,10 +16225,10 @@
     </row>
     <row r="38" spans="3:6" ht="32" x14ac:dyDescent="0.2">
       <c r="C38" s="8" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="D38" s="29" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F38" t="b">
         <v>0</v>
@@ -15210,7 +16236,7 @@
     </row>
     <row r="39" spans="3:6" ht="32" x14ac:dyDescent="0.2">
       <c r="C39" s="8" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="D39" s="29" t="s">
         <v>33</v>
@@ -15221,7 +16247,7 @@
     </row>
     <row r="40" spans="3:6" ht="16" x14ac:dyDescent="0.2">
       <c r="C40" s="8" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="D40" s="29" t="s">
         <v>73</v>
@@ -15235,7 +16261,7 @@
         <v>16</v>
       </c>
       <c r="D42" s="23" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="43" spans="3:6" ht="16" x14ac:dyDescent="0.2">
@@ -15254,7 +16280,7 @@
         <v>5</v>
       </c>
       <c r="D44" s="29" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F44" t="b">
         <v>0</v>
@@ -15262,10 +16288,10 @@
     </row>
     <row r="45" spans="3:6" ht="16" x14ac:dyDescent="0.2">
       <c r="C45" s="8" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="D45" s="29" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F45" t="b">
         <v>0</v>
@@ -15273,10 +16299,10 @@
     </row>
     <row r="46" spans="3:6" ht="16" x14ac:dyDescent="0.2">
       <c r="C46" s="8" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="D46" s="29" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F46" t="b">
         <v>0</v>
@@ -15287,7 +16313,7 @@
         <v>5</v>
       </c>
       <c r="D47" s="29" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F47" t="b">
         <v>0</v>
@@ -15295,10 +16321,10 @@
     </row>
     <row r="48" spans="3:6" ht="16" x14ac:dyDescent="0.2">
       <c r="C48" s="8" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="D48" s="29" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F48" t="b">
         <v>0</v>
@@ -15306,10 +16332,10 @@
     </row>
     <row r="49" spans="3:6" ht="16" x14ac:dyDescent="0.2">
       <c r="C49" s="8" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="D49" s="29" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F49" t="b">
         <v>0</v>
@@ -15331,7 +16357,7 @@
         <v>5</v>
       </c>
       <c r="D52" s="35" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="F52" t="b">
         <v>0</v>
@@ -15339,10 +16365,10 @@
     </row>
     <row r="53" spans="3:6" ht="16" x14ac:dyDescent="0.2">
       <c r="C53" s="8" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="D53" s="35" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="F53" t="b">
         <v>0</v>
@@ -15350,10 +16376,10 @@
     </row>
     <row r="54" spans="3:6" ht="16" x14ac:dyDescent="0.2">
       <c r="C54" s="8" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="D54" s="35" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="F54" t="b">
         <v>0</v>
@@ -15361,10 +16387,10 @@
     </row>
     <row r="55" spans="3:6" ht="16" x14ac:dyDescent="0.2">
       <c r="C55" s="8" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D55" s="35" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="F55" t="b">
         <v>0</v>
@@ -15372,10 +16398,10 @@
     </row>
     <row r="56" spans="3:6" ht="16" x14ac:dyDescent="0.2">
       <c r="C56" s="8" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="D56" s="35" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="F56" t="b">
         <v>0</v>
@@ -15386,7 +16412,7 @@
         <v>5</v>
       </c>
       <c r="D57" s="35" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="F57" t="b">
         <v>0</v>
@@ -15394,10 +16420,10 @@
     </row>
     <row r="58" spans="3:6" ht="16" x14ac:dyDescent="0.2">
       <c r="C58" s="8" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="D58" s="35" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="F58" t="b">
         <v>0</v>
@@ -15405,10 +16431,10 @@
     </row>
     <row r="59" spans="3:6" ht="16" x14ac:dyDescent="0.2">
       <c r="C59" s="8" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="D59" s="35" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="F59" t="b">
         <v>0</v>
@@ -15416,10 +16442,10 @@
     </row>
     <row r="60" spans="3:6" ht="16" x14ac:dyDescent="0.2">
       <c r="C60" s="8" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="D60" s="35" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="F60" t="b">
         <v>0</v>
@@ -15427,10 +16453,10 @@
     </row>
     <row r="61" spans="3:6" ht="16" x14ac:dyDescent="0.2">
       <c r="C61" s="8" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="D61" s="35" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="F61" t="b">
         <v>0</v>
@@ -15449,7 +16475,7 @@
         <v>5</v>
       </c>
       <c r="D64" s="35" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="F64" t="b">
         <v>0</v>
@@ -15457,10 +16483,10 @@
     </row>
     <row r="65" spans="3:6" ht="16" x14ac:dyDescent="0.2">
       <c r="C65" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="D65" s="35" t="s">
         <v>163</v>
-      </c>
-      <c r="D65" s="35" t="s">
-        <v>169</v>
       </c>
       <c r="F65" t="b">
         <v>0</v>
@@ -15468,10 +16494,10 @@
     </row>
     <row r="66" spans="3:6" ht="16" x14ac:dyDescent="0.2">
       <c r="C66" s="8" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="D66" s="35" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="F66" t="b">
         <v>0</v>
@@ -15482,7 +16508,7 @@
         <v>5</v>
       </c>
       <c r="D67" s="35" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="F67" t="b">
         <v>0</v>
@@ -15490,10 +16516,10 @@
     </row>
     <row r="68" spans="3:6" ht="16" x14ac:dyDescent="0.2">
       <c r="C68" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="D68" s="35" t="s">
         <v>163</v>
-      </c>
-      <c r="D68" s="35" t="s">
-        <v>169</v>
       </c>
       <c r="F68" t="b">
         <v>0</v>
@@ -15501,10 +16527,10 @@
     </row>
     <row r="69" spans="3:6" ht="16" x14ac:dyDescent="0.2">
       <c r="C69" s="8" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="D69" s="35" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="F69" t="b">
         <v>0</v>
@@ -15515,15 +16541,15 @@
         <v>16</v>
       </c>
       <c r="D71" s="27" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
     </row>
     <row r="72" spans="3:6" ht="16" x14ac:dyDescent="0.2">
       <c r="C72" s="8" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D72" s="35" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="F72" t="b">
         <v>0</v>
@@ -15534,7 +16560,7 @@
         <v>5</v>
       </c>
       <c r="D73" s="35" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="F73" t="b">
         <v>0</v>
@@ -15542,10 +16568,10 @@
     </row>
     <row r="74" spans="3:6" ht="16" x14ac:dyDescent="0.2">
       <c r="C74" s="8" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="D74" s="35" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="F74" t="b">
         <v>0</v>
@@ -15556,7 +16582,7 @@
         <v>5</v>
       </c>
       <c r="D75" s="35" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="F75" t="b">
         <v>0</v>
@@ -15564,10 +16590,10 @@
     </row>
     <row r="76" spans="3:6" ht="16" x14ac:dyDescent="0.2">
       <c r="C76" s="8" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="D76" s="35" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="F76" t="b">
         <v>0</v>
@@ -15575,7 +16601,7 @@
     </row>
     <row r="78" spans="3:6" ht="16" x14ac:dyDescent="0.2">
       <c r="C78" s="18" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
     </row>
     <row r="79" spans="3:6" ht="16" x14ac:dyDescent="0.2">
@@ -15583,12 +16609,12 @@
         <v>16</v>
       </c>
       <c r="D79" s="44" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="80" spans="3:6" ht="16" x14ac:dyDescent="0.2">
       <c r="C80" s="8" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="D80" s="29" t="s">
         <v>36</v>
@@ -15599,24 +16625,24 @@
     </row>
     <row r="81" spans="3:7" ht="48" x14ac:dyDescent="0.2">
       <c r="C81" s="8" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="D81" s="35" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="F81" t="b">
         <v>0</v>
       </c>
       <c r="G81" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
     </row>
     <row r="82" spans="3:7" ht="48" x14ac:dyDescent="0.2">
       <c r="C82" s="8" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="D82" s="35" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="F82" t="b">
         <v>0</v>
@@ -15624,10 +16650,10 @@
     </row>
     <row r="83" spans="3:7" ht="16" x14ac:dyDescent="0.2">
       <c r="C83" s="8" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="D83" s="35" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="F83" t="b">
         <v>0</v>
@@ -15635,10 +16661,10 @@
     </row>
     <row r="84" spans="3:7" ht="48" x14ac:dyDescent="0.2">
       <c r="C84" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="D84" s="35" t="s">
         <v>229</v>
-      </c>
-      <c r="D84" s="35" t="s">
-        <v>235</v>
       </c>
       <c r="F84" t="b">
         <v>0</v>
@@ -15647,7 +16673,7 @@
     <row r="85" spans="3:7" ht="32" x14ac:dyDescent="0.2">
       <c r="C85" s="8"/>
       <c r="D85" s="35" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="F85" t="b">
         <v>0</v>
@@ -15663,7 +16689,7 @@
     </row>
     <row r="88" spans="3:7" ht="16" x14ac:dyDescent="0.2">
       <c r="C88" s="8" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="D88" s="29" t="s">
         <v>36</v>
@@ -15674,10 +16700,10 @@
     </row>
     <row r="89" spans="3:7" ht="32" x14ac:dyDescent="0.2">
       <c r="C89" s="8" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="D89" s="35" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="F89" t="b">
         <v>0</v>
@@ -15685,66 +16711,66 @@
     </row>
     <row r="90" spans="3:7" ht="32" x14ac:dyDescent="0.2">
       <c r="C90" s="8" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="D90" s="35" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="F90" t="b">
         <v>0</v>
       </c>
       <c r="G90" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
     </row>
     <row r="91" spans="3:7" ht="32" x14ac:dyDescent="0.2">
       <c r="C91" s="8" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="D91" s="35" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
     </row>
     <row r="92" spans="3:7" ht="32" x14ac:dyDescent="0.2">
       <c r="C92" s="8"/>
       <c r="D92" s="35" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
     </row>
     <row r="93" spans="3:7" ht="32" x14ac:dyDescent="0.2">
       <c r="C93" s="8" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="D93" s="35" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
     </row>
     <row r="94" spans="3:7" ht="32" x14ac:dyDescent="0.2">
       <c r="C94" s="8"/>
       <c r="D94" s="35" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
     </row>
     <row r="95" spans="3:7" ht="48" x14ac:dyDescent="0.2">
       <c r="C95" s="8" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="D95" s="35" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
     </row>
     <row r="96" spans="3:7" ht="32" x14ac:dyDescent="0.2">
       <c r="C96" s="8" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="D96" s="35" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
     </row>
     <row r="97" spans="3:6" ht="32" x14ac:dyDescent="0.2">
       <c r="C97" s="8"/>
       <c r="D97" s="35" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
     </row>
     <row r="99" spans="3:6" ht="16" x14ac:dyDescent="0.2">
@@ -15757,28 +16783,28 @@
     </row>
     <row r="100" spans="3:6" ht="32" x14ac:dyDescent="0.2">
       <c r="C100" s="8" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="D100" s="35" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
     </row>
     <row r="101" spans="3:6" ht="32" x14ac:dyDescent="0.2">
       <c r="C101" s="8"/>
       <c r="D101" s="35" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
     </row>
     <row r="102" spans="3:6" ht="32" x14ac:dyDescent="0.2">
       <c r="C102" s="8"/>
       <c r="D102" s="35" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
     </row>
     <row r="103" spans="3:6" ht="32" x14ac:dyDescent="0.2">
       <c r="C103" s="8"/>
       <c r="D103" s="35" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
     </row>
     <row r="105" spans="3:6" ht="16" x14ac:dyDescent="0.2">
@@ -15786,12 +16812,12 @@
         <v>16</v>
       </c>
       <c r="D105" s="44" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
     </row>
     <row r="106" spans="3:6" ht="16" x14ac:dyDescent="0.2">
       <c r="C106" s="8" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="D106" s="29" t="s">
         <v>36</v>
@@ -15802,7 +16828,7 @@
     </row>
     <row r="107" spans="3:6" ht="64" x14ac:dyDescent="0.2">
       <c r="C107" s="8" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="D107" s="29" t="s">
         <v>37</v>
@@ -15813,7 +16839,7 @@
     </row>
     <row r="108" spans="3:6" ht="32" x14ac:dyDescent="0.2">
       <c r="C108" s="8" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="D108" s="29" t="s">
         <v>38</v>
@@ -15821,48 +16847,48 @@
     </row>
     <row r="112" spans="3:6" ht="16" x14ac:dyDescent="0.2">
       <c r="D112" s="28" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
     </row>
     <row r="113" spans="4:5" ht="16" x14ac:dyDescent="0.2">
       <c r="D113" s="25" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
     </row>
     <row r="114" spans="4:5" ht="16" x14ac:dyDescent="0.2">
       <c r="D114" s="25" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="115" spans="4:5" ht="16" x14ac:dyDescent="0.2">
       <c r="D115" s="25" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
     </row>
     <row r="116" spans="4:5" ht="16" x14ac:dyDescent="0.2">
       <c r="D116" s="25" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
     </row>
     <row r="117" spans="4:5" ht="32" x14ac:dyDescent="0.2">
       <c r="D117" s="25" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
     </row>
     <row r="118" spans="4:5" ht="16" x14ac:dyDescent="0.2">
       <c r="D118" s="25" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
     </row>
     <row r="121" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D121" s="42" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="E121" s="43"/>
     </row>
     <row r="123" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D123" s="42" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="E123" s="43"/>
     </row>
@@ -15873,107 +16899,107 @@
   </mergeCells>
   <phoneticPr fontId="20" type="noConversion"/>
   <conditionalFormatting sqref="D7:D14">
-    <cfRule type="expression" dxfId="25" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="26" stopIfTrue="1">
       <formula>AND($F7=FALSE,$F6&lt;&gt;FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="30">
+    <cfRule type="expression" dxfId="28" priority="30">
       <formula>$F7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D17:D22">
-    <cfRule type="expression" dxfId="23" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="24" stopIfTrue="1">
       <formula>AND($F17=FALSE,$F16&lt;&gt;FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="25">
+    <cfRule type="expression" dxfId="26" priority="25">
       <formula>$F17</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D26:D28">
-    <cfRule type="expression" dxfId="21" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="21" stopIfTrue="1">
       <formula>AND($F26=FALSE,$F25&lt;&gt;FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="22">
+    <cfRule type="expression" dxfId="24" priority="22">
       <formula>$F26</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D31:D33">
-    <cfRule type="expression" dxfId="19" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="19" stopIfTrue="1">
       <formula>AND($F31=FALSE,$F30&lt;&gt;FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="20">
+    <cfRule type="expression" dxfId="22" priority="20">
       <formula>$F31</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D36:D40">
-    <cfRule type="expression" dxfId="17" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="17" stopIfTrue="1">
       <formula>AND($F36=FALSE,$F35&lt;&gt;FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="18">
+    <cfRule type="expression" dxfId="20" priority="18">
       <formula>$F36</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D43:D49">
-    <cfRule type="expression" dxfId="15" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="15" stopIfTrue="1">
       <formula>AND($F43=FALSE,$F42&lt;&gt;FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="16">
+    <cfRule type="expression" dxfId="18" priority="16">
       <formula>$F43</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D52:D61">
-    <cfRule type="expression" dxfId="13" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="13" stopIfTrue="1">
       <formula>AND($F52=FALSE,$F51&lt;&gt;FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="14">
+    <cfRule type="expression" dxfId="16" priority="14">
       <formula>$F52</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D64:D69">
-    <cfRule type="expression" dxfId="11" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="11" stopIfTrue="1">
       <formula>AND($F64=FALSE,$F63&lt;&gt;FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="12">
+    <cfRule type="expression" dxfId="14" priority="12">
       <formula>$F64</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D72:D76">
-    <cfRule type="expression" dxfId="9" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="9" stopIfTrue="1">
       <formula>AND($F72=FALSE,$F71&lt;&gt;FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="10">
+    <cfRule type="expression" dxfId="12" priority="10">
       <formula>$F72</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D80:D85">
-    <cfRule type="expression" dxfId="7" priority="8">
+    <cfRule type="expression" dxfId="11" priority="7" stopIfTrue="1">
+      <formula>AND($F80=FALSE,$F79&lt;&gt;FALSE)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="8">
       <formula>$F80</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="6" priority="7" stopIfTrue="1">
-      <formula>AND($F80=FALSE,$F79&lt;&gt;FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D88:D97">
-    <cfRule type="expression" dxfId="5" priority="6">
+    <cfRule type="expression" dxfId="9" priority="5" stopIfTrue="1">
+      <formula>AND($F88=FALSE,$F87&lt;&gt;FALSE)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="8" priority="6">
       <formula>$F88</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="4" priority="5" stopIfTrue="1">
-      <formula>AND($F88=FALSE,$F87&lt;&gt;FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D100:D103">
-    <cfRule type="expression" dxfId="2" priority="4">
+    <cfRule type="expression" dxfId="7" priority="3" stopIfTrue="1">
+      <formula>AND($F100=FALSE,$F99&lt;&gt;FALSE)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="4">
       <formula>$F100</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="3" stopIfTrue="1">
-      <formula>AND($F100=FALSE,$F99&lt;&gt;FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D106:D108">
-    <cfRule type="expression" dxfId="3" priority="2">
+    <cfRule type="expression" dxfId="5" priority="1" stopIfTrue="1">
+      <formula>AND($F106=FALSE,$F105&lt;&gt;FALSE)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="2">
       <formula>$F106</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
-      <formula>AND($F106=FALSE,$F105&lt;&gt;FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -17700,7 +18726,7 @@
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D2" s="37" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="E2" s="38"/>
       <c r="F2" t="b">
@@ -17709,16 +18735,16 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="16" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B3" s="16" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -17726,7 +18752,7 @@
         <v>14</v>
       </c>
       <c r="F4" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="48.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -17734,7 +18760,7 @@
         <v>7</v>
       </c>
       <c r="D6" s="39" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="32.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -17742,7 +18768,7 @@
         <v>7</v>
       </c>
       <c r="D7" s="39" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -17750,7 +18776,7 @@
         <v>7</v>
       </c>
       <c r="D8" s="40" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>